<commit_message>
refactor: calculation period has been changed
</commit_message>
<xml_diff>
--- a/ServiceJob/JVNLP_.xlsx
+++ b/ServiceJob/JVNLP_.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ЖВНЛП" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>МНН</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Дата вступления в силу</t>
+  </si>
+  <si>
+    <t>Причина исключения</t>
+  </si>
+  <si>
+    <t>Дата исключения</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -358,6 +364,12 @@
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -375,12 +387,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,6 +414,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -718,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
@@ -745,39 +762,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="21"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="29" t="s">
@@ -786,19 +803,19 @@
       <c r="G2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="24" t="s">
@@ -817,18 +834,18 @@
       <c r="R2" s="28"/>
     </row>
     <row r="3" spans="1:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="30"/>
       <c r="G3" s="25"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="20"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
@@ -847,6 +864,7 @@
     <sortCondition ref="A4:A39847"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A1:R1"/>
@@ -863,7 +881,6 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -904,39 +921,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="21"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="29" t="s">
@@ -945,19 +962,19 @@
       <c r="G2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="24" t="s">
@@ -976,18 +993,18 @@
       <c r="R2" s="28"/>
     </row>
     <row r="3" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="30"/>
       <c r="G3" s="25"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="20"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
@@ -1006,6 +1023,7 @@
     <sortCondition ref="A4:A625"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="N2:N3"/>
@@ -1022,7 +1040,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1034,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1053,12 +1070,12 @@
     <col min="9" max="9" width="11.5703125" style="10" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" style="15" customWidth="1"/>
     <col min="11" max="11" width="12" style="10" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="35" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="16" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -1071,8 +1088,9 @@
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
     </row>
-    <row r="2" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1106,8 +1124,11 @@
       <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>18</v>
+      <c r="L2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>